<commit_message>
Query Store - Regressed Queries
</commit_message>
<xml_diff>
--- a/Monitoring Solutions/Availability Groups Monitoring/AG Monitoring Design.xlsx
+++ b/Monitoring Solutions/Availability Groups Monitoring/AG Monitoring Design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://madeira844.sharepoint.com/sites/Everyone/Shared Documents/Professional Resources/Madeira Toolbox/Monitoring Solutions/Availability Groups Monitoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB9BC88-5FB6-4691-8099-C3EB4FE95525}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB9BC88-5FB6-4691-8099-C3EB4FE95525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18448" yWindow="-1589" windowWidth="26301" windowHeight="14304" xr2:uid="{9B040424-B504-4714-8EE2-EB47C31A3A48}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B040424-B504-4714-8EE2-EB47C31A3A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Architecture" sheetId="3" r:id="rId1"/>
@@ -326,13 +326,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -471,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -482,12 +489,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -503,44 +510,47 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -858,42 +868,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E182243F-419C-44FD-9B7C-2B3726F1117B}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="22.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="105.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="37.375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="69.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.64453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.76171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="105.46875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="37.3515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="69.64453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.64453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.64453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.87890625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="21"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="11" t="s">
         <v>8</v>
       </c>
@@ -904,7 +914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="100.55" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="100.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
@@ -915,7 +925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="114.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="100.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
@@ -926,29 +936,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="100.55" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="100.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="23" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="100.55" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="100.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
@@ -959,98 +969,98 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:5" ht="72" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="100.55" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:5" ht="115" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" s="2"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" s="2"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" s="2"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" s="2"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" s="2"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" s="2"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" s="2"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" s="2"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" s="2"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1064,21 +1074,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A0B9F8B3991C594AB7A558D53E9A462C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="933955d8f081e12cb87b134a0e779cf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1c853891-79e1-4665-8425-27cfb243d1fd" xmlns:ns3="c8f11c67-c3b6-4b83-8087-70e71e9ec41f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c60842fcf194f8ef6378e3100f4700a" ns2:_="" ns3:_="">
     <xsd:import namespace="1c853891-79e1-4665-8425-27cfb243d1fd"/>
@@ -1301,10 +1296,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33CBE407-A537-44AE-A015-1468E5EFE58B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9AD1F90-C9FA-444E-B375-991C34C6359B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1c853891-79e1-4665-8425-27cfb243d1fd"/>
+    <ds:schemaRef ds:uri="c8f11c67-c3b6-4b83-8087-70e71e9ec41f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1319,5 +1340,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9AD1F90-C9FA-444E-B375-991C34C6359B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33CBE407-A537-44AE-A015-1468E5EFE58B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>